<commit_message>
Uppfæri gögn frá seðlabankanum
</commit_message>
<xml_diff>
--- a/data/Verdbolguvaentingar-a-mismunandi-maelikvarda.xlsx
+++ b/data/Verdbolguvaentingar-a-mismunandi-maelikvarda.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29728"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E22569C-C715-48B0-8437-49523F558166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D70FD86-4804-4F3F-88F6-43535411B338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25260" yWindow="21600" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20025" yWindow="2580" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heimili_Households" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentManualCount="32"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="122">
   <si>
     <t>Verðbólguvæntingar heimila / Household inflation expectations</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>2025Q3</t>
+  </si>
+  <si>
+    <t>2025Q4</t>
   </si>
   <si>
     <t>Meðaltal / average</t>
@@ -450,64 +453,16 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Verðbólguálag til 1 árs / 1-year breakeven rate</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Verðbólguálag til 2 ára / 2-year breakeven rate</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Verðbólguálag til 5 ára / 5-year breakeven rate</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Verðbólguálag til 10 ára / 10-year breakeven rate</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
+    <t>Verðbólguálag til 1 árs / 1-year breakeven rate</t>
+  </si>
+  <si>
+    <t>Verðbólguálag til 2 ára / 2-year breakeven rate</t>
+  </si>
+  <si>
+    <t>Verðbólguálag til 5 ára / 5-year breakeven rate</t>
+  </si>
+  <si>
+    <t>Verðbólguálag til 10 ára / 10-year breakeven rate</t>
   </si>
   <si>
     <t>1. Ársfjórðungsleg meðaltöl. Verðbólguálagið er reiknað út frá vaxtamun verðtryggðra og óverðtryggðra skuldabréfa. Við túlkun þess þarf að hafa í huga að það inniheldur einnig áhættuálag sem tengist seljanleika bréfanna auk áhættuálags vegna óvissu um verðbólgu.</t>
@@ -522,31 +477,6 @@
       </rPr>
       <t xml:space="preserve">1. Quarterly averages. The breakeven inflation rate is calculated from the spread between indexed and nominal bond interest rates. It should be borne in mind, however, that the breakeven rate also includes a liquidity risk premium and an inflation risk premium.  </t>
     </r>
-  </si>
-  <si>
-    <t>2. Við mat á eingreiðsluferli verðtryggðra og óverðtryggðra vaxta notast
-Seðlabankinn við aðferð Nelson-Siegel. Matið á verðtryggða vaxtaferlinum
-hefur í vaxandi mæli litast af ávöxtun skuldabréfs sem er á
-gjalddaga snemma á næsta ári og datt út úr viðskiptavakt um miðjan
-ágúst. Bréfið hefur valdið því að verðtryggðir eingreiðsluvextir hafa
-undanfarið mælst of háir miðað við fyrirliggjandi meðallöng verðtryggð
-skuldabréf og þannig leitt til vanmats á verðbólguálagi á skuldabréfamarkaði
-til skemmri og meðallangs tíma. Til að laga þetta hefur þetta
-skuldabréf verið tekið út úr matinu frá því í maí í fyrra sem hefur áhrif á
-söguleg gögn um verðbólguálagið og metna raunvexti út frá álaginu.</t>
-  </si>
-  <si>
-    <t>2. The indexed and non-indexed zero-coupon yield curves are estimated
-using the Nelson-Siegel method. The estimation of the indexed yield
-curve has increasingly been affected by yields on a bond maturing
-in early 2026, for which market making was discontinued as of mid-
-August. This bond has caused indexed zero-coupon rates to measure
-excessively high in terms of current medium-term indexed bonds,
-thereby leading to an underestimation of the short- and medium-term
-breakeven inflation rate in the bond market. In order to correct for this,
-the bond in question was removed from the estimation from May 2024
-onwards, which affects historical data on both the breakeven rate and
-the real rate as estimated from the breakeven rate.</t>
   </si>
   <si>
     <r>
@@ -577,7 +507,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,13 +612,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -1057,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CN35"/>
+  <dimension ref="A1:CO35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CL1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="CJ1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -1076,10 +999,10 @@
     <col min="49" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" ht="17.25">
+    <row r="1" spans="1:93" ht="17.25">
       <c r="A1" s="8"/>
     </row>
-    <row r="2" spans="1:92">
+    <row r="2" spans="1:93">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1128,28 +1051,28 @@
       <c r="AR2" s="10"/>
       <c r="AS2" s="10"/>
     </row>
-    <row r="3" spans="1:92" ht="17.25">
+    <row r="3" spans="1:93" ht="17.25">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:92">
+    <row r="4" spans="1:93">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:92">
+    <row r="5" spans="1:93">
       <c r="A5" s="11"/>
     </row>
-    <row r="6" spans="1:92">
+    <row r="6" spans="1:93">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:92">
+    <row r="7" spans="1:93">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:92">
+    <row r="8" spans="1:93">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
@@ -1234,8 +1157,9 @@
       <c r="CL8" s="15"/>
       <c r="CM8" s="15"/>
       <c r="CN8" s="15"/>
+      <c r="CO8" s="15"/>
     </row>
-    <row r="9" spans="1:92">
+    <row r="9" spans="1:93">
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1287,7 +1211,7 @@
       <c r="BZ9" s="16"/>
       <c r="CA9" s="16"/>
     </row>
-    <row r="10" spans="1:92">
+    <row r="10" spans="1:93">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1561,10 +1485,13 @@
       <c r="CN10" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="CO10" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="11" spans="1:92">
+    <row r="11" spans="1:93">
       <c r="A11" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B11" s="5">
         <v>3.6</v>
@@ -1839,10 +1766,13 @@
       <c r="CN11" s="2">
         <v>5.5</v>
       </c>
+      <c r="CO11" s="2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="12" spans="1:92">
+    <row r="12" spans="1:93">
       <c r="A12" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B12" s="5">
         <v>3</v>
@@ -2117,10 +2047,13 @@
       <c r="CN12" s="2">
         <v>4.5</v>
       </c>
+      <c r="CO12" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="13" spans="1:92">
+    <row r="13" spans="1:93">
       <c r="A13" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B13" s="5">
         <v>2.5</v>
@@ -2395,8 +2328,11 @@
       <c r="CN13" s="2">
         <v>3</v>
       </c>
+      <c r="CO13" s="2">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
-    <row r="14" spans="1:92">
+    <row r="14" spans="1:93">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -2483,8 +2419,9 @@
       <c r="CL14" s="15"/>
       <c r="CM14" s="15"/>
       <c r="CN14" s="15"/>
+      <c r="CO14" s="15"/>
     </row>
-    <row r="15" spans="1:92">
+    <row r="15" spans="1:93">
       <c r="BV15" s="16"/>
       <c r="BW15" s="16"/>
       <c r="BX15" s="16"/>
@@ -2492,19 +2429,19 @@
       <c r="BZ15" s="16"/>
       <c r="CA15" s="16"/>
     </row>
-    <row r="16" spans="1:92">
+    <row r="16" spans="1:93">
       <c r="A16" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:92">
+    <row r="17" spans="1:93">
       <c r="A17" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:92">
+    <row r="18" spans="1:93">
       <c r="A18" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -2586,8 +2523,9 @@
       <c r="CL18" s="15"/>
       <c r="CM18" s="15"/>
       <c r="CN18" s="15"/>
+      <c r="CO18" s="15"/>
     </row>
-    <row r="19" spans="1:92">
+    <row r="19" spans="1:93">
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
@@ -2640,7 +2578,7 @@
       <c r="CA19" s="16"/>
       <c r="CB19" s="16"/>
     </row>
-    <row r="20" spans="1:92">
+    <row r="20" spans="1:93">
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
@@ -2914,10 +2852,13 @@
       <c r="CN20" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="CO20" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="21" spans="1:92">
+    <row r="21" spans="1:93">
       <c r="A21" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -3146,10 +3087,13 @@
       <c r="CN21" s="2">
         <v>5.3</v>
       </c>
+      <c r="CO21" s="2">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="22" spans="1:92">
+    <row r="22" spans="1:93">
       <c r="A22" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -3378,10 +3322,13 @@
       <c r="CN22" s="2">
         <v>4</v>
       </c>
+      <c r="CO22" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:92">
+    <row r="23" spans="1:93">
       <c r="A23" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -3610,8 +3557,11 @@
       <c r="CN23" s="2">
         <v>3.2</v>
       </c>
+      <c r="CO23" s="2">
+        <v>2.8</v>
+      </c>
     </row>
-    <row r="24" spans="1:92">
+    <row r="24" spans="1:93">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -3697,8 +3647,9 @@
       <c r="CL24" s="15"/>
       <c r="CM24" s="15"/>
       <c r="CN24" s="15"/>
+      <c r="CO24" s="15"/>
     </row>
-    <row r="25" spans="1:92">
+    <row r="25" spans="1:93">
       <c r="BV25" s="16"/>
       <c r="BW25" s="16"/>
       <c r="BX25" s="16"/>
@@ -3707,19 +3658,19 @@
       <c r="CA25" s="16"/>
       <c r="CB25" s="16"/>
     </row>
-    <row r="26" spans="1:92">
+    <row r="26" spans="1:93">
       <c r="A26" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:92">
+    <row r="27" spans="1:93">
       <c r="A27" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:92">
+    <row r="28" spans="1:93">
       <c r="A28" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -3801,8 +3752,9 @@
       <c r="CL28" s="15"/>
       <c r="CM28" s="15"/>
       <c r="CN28" s="15"/>
+      <c r="CO28" s="15"/>
     </row>
-    <row r="29" spans="1:92">
+    <row r="29" spans="1:93">
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
@@ -3855,7 +3807,7 @@
       <c r="CA29" s="16"/>
       <c r="CB29" s="16"/>
     </row>
-    <row r="30" spans="1:92">
+    <row r="30" spans="1:93">
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
@@ -4129,10 +4081,13 @@
       <c r="CN30" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="CO30" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="31" spans="1:92">
+    <row r="31" spans="1:93">
       <c r="A31" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -4287,10 +4242,13 @@
       <c r="CN31" s="2">
         <v>5.0999999999999996</v>
       </c>
+      <c r="CO31" s="2">
+        <v>4.5999999999999996</v>
+      </c>
     </row>
-    <row r="32" spans="1:92">
+    <row r="32" spans="1:93">
       <c r="A32" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -4445,10 +4403,13 @@
       <c r="CN32" s="2">
         <v>4</v>
       </c>
+      <c r="CO32" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="33" spans="1:92">
+    <row r="33" spans="1:93">
       <c r="A33" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -4603,8 +4564,11 @@
       <c r="CN33" s="2">
         <v>2.8</v>
       </c>
+      <c r="CO33" s="2">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
-    <row r="34" spans="1:92">
+    <row r="34" spans="1:93">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -4690,10 +4654,11 @@
       <c r="CL34" s="15"/>
       <c r="CM34" s="15"/>
       <c r="CN34" s="15"/>
+      <c r="CO34" s="15"/>
     </row>
-    <row r="35" spans="1:92">
+    <row r="35" spans="1:93">
       <c r="A35" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BV35" s="16"/>
       <c r="BW35" s="16"/>
@@ -4712,9 +4677,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:CN39"/>
+  <dimension ref="A1:CO39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CJ1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
@@ -4731,12 +4696,12 @@
     <col min="49" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" ht="17.25">
+    <row r="1" spans="1:93" ht="17.25">
       <c r="A1" s="8"/>
     </row>
-    <row r="2" spans="1:92">
+    <row r="2" spans="1:93">
       <c r="A2" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4783,30 +4748,30 @@
       <c r="AR2" s="10"/>
       <c r="AS2" s="10"/>
     </row>
-    <row r="3" spans="1:92" ht="17.25">
+    <row r="3" spans="1:93" ht="17.25">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:92">
+    <row r="4" spans="1:93">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:92">
+    <row r="5" spans="1:93">
       <c r="A5" s="11"/>
     </row>
-    <row r="6" spans="1:92">
+    <row r="6" spans="1:93">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:92">
+    <row r="7" spans="1:93">
       <c r="A7" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:92">
+    <row r="8" spans="1:93">
       <c r="A8" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -4889,8 +4854,9 @@
       <c r="CL8" s="15"/>
       <c r="CM8" s="15"/>
       <c r="CN8" s="15"/>
+      <c r="CO8" s="15"/>
     </row>
-    <row r="9" spans="1:92">
+    <row r="9" spans="1:93">
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
@@ -4942,7 +4908,7 @@
       <c r="CA9" s="16"/>
       <c r="CB9" s="16"/>
     </row>
-    <row r="10" spans="1:92">
+    <row r="10" spans="1:93">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -5216,10 +5182,13 @@
       <c r="CN10" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="CO10" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="11" spans="1:92">
+    <row r="11" spans="1:93">
       <c r="A11" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B11" s="5">
         <v>2.1</v>
@@ -5480,10 +5449,13 @@
       <c r="CN11" s="2">
         <v>4.2</v>
       </c>
+      <c r="CO11" s="2">
+        <v>4.2</v>
+      </c>
     </row>
-    <row r="12" spans="1:92">
+    <row r="12" spans="1:93">
       <c r="A12" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
@@ -5742,10 +5714,13 @@
       <c r="CN12" s="2">
         <v>4</v>
       </c>
+      <c r="CO12" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="13" spans="1:92">
+    <row r="13" spans="1:93">
       <c r="A13" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B13" s="5">
         <v>1.9</v>
@@ -6006,8 +5981,11 @@
       <c r="CN13" s="2">
         <v>1.1000000000000001</v>
       </c>
+      <c r="CO13" s="2">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
-    <row r="14" spans="1:92">
+    <row r="14" spans="1:93">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -6093,8 +6071,9 @@
       <c r="CL14" s="15"/>
       <c r="CM14" s="15"/>
       <c r="CN14" s="15"/>
+      <c r="CO14" s="15"/>
     </row>
-    <row r="15" spans="1:92">
+    <row r="15" spans="1:93">
       <c r="BV15" s="16"/>
       <c r="BW15" s="16"/>
       <c r="BX15" s="16"/>
@@ -6103,19 +6082,19 @@
       <c r="CA15" s="16"/>
       <c r="CB15" s="16"/>
     </row>
-    <row r="16" spans="1:92">
+    <row r="16" spans="1:93">
       <c r="A16" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:92">
+    <row r="17" spans="1:93">
       <c r="A17" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:92">
+    <row r="18" spans="1:93">
       <c r="A18" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -6199,8 +6178,9 @@
       <c r="CL18" s="15"/>
       <c r="CM18" s="15"/>
       <c r="CN18" s="15"/>
+      <c r="CO18" s="15"/>
     </row>
-    <row r="19" spans="1:92">
+    <row r="19" spans="1:93">
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
@@ -6251,7 +6231,7 @@
       <c r="CA19" s="16"/>
       <c r="CB19" s="16"/>
     </row>
-    <row r="20" spans="1:92">
+    <row r="20" spans="1:93">
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
@@ -6525,10 +6505,13 @@
       <c r="CN20" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="CO20" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="21" spans="1:92">
+    <row r="21" spans="1:93">
       <c r="A21" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -6725,10 +6708,13 @@
       <c r="CN21" s="2">
         <v>4</v>
       </c>
+      <c r="CO21" s="2">
+        <v>3.9</v>
+      </c>
     </row>
-    <row r="22" spans="1:92">
+    <row r="22" spans="1:93">
       <c r="A22" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -6925,10 +6911,13 @@
       <c r="CN22" s="2">
         <v>3.5</v>
       </c>
+      <c r="CO22" s="2">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="23" spans="1:92">
+    <row r="23" spans="1:93">
       <c r="A23" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -7125,8 +7114,11 @@
       <c r="CN23" s="2">
         <v>1.5</v>
       </c>
+      <c r="CO23" s="2">
+        <v>1.3</v>
+      </c>
     </row>
-    <row r="24" spans="1:92">
+    <row r="24" spans="1:93">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -7212,8 +7204,9 @@
       <c r="CL24" s="15"/>
       <c r="CM24" s="15"/>
       <c r="CN24" s="15"/>
+      <c r="CO24" s="15"/>
     </row>
-    <row r="25" spans="1:92">
+    <row r="25" spans="1:93">
       <c r="BV25" s="16"/>
       <c r="BW25" s="16"/>
       <c r="BX25" s="16"/>
@@ -7222,19 +7215,19 @@
       <c r="CA25" s="16"/>
       <c r="CB25" s="16"/>
     </row>
-    <row r="26" spans="1:92">
+    <row r="26" spans="1:93">
       <c r="A26" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:92">
+    <row r="27" spans="1:93">
       <c r="A27" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:92">
+    <row r="28" spans="1:93">
       <c r="A28" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -7318,8 +7311,9 @@
       <c r="CL28" s="15"/>
       <c r="CM28" s="15"/>
       <c r="CN28" s="15"/>
+      <c r="CO28" s="15"/>
     </row>
-    <row r="29" spans="1:92">
+    <row r="29" spans="1:93">
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
@@ -7370,7 +7364,7 @@
       <c r="CA29" s="16"/>
       <c r="CB29" s="16"/>
     </row>
-    <row r="30" spans="1:92">
+    <row r="30" spans="1:93">
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
@@ -7644,10 +7638,13 @@
       <c r="CN30" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="CO30" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="31" spans="1:92">
+    <row r="31" spans="1:93">
       <c r="A31" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -7800,10 +7797,13 @@
       <c r="CN31" s="2">
         <v>3.9</v>
       </c>
+      <c r="CO31" s="2">
+        <v>3.8</v>
+      </c>
     </row>
-    <row r="32" spans="1:92">
+    <row r="32" spans="1:93">
       <c r="A32" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -7956,10 +7956,13 @@
       <c r="CN32" s="2">
         <v>3.5</v>
       </c>
+      <c r="CO32" s="2">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="33" spans="1:92">
+    <row r="33" spans="1:93">
       <c r="A33" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -8112,8 +8115,11 @@
       <c r="CN33" s="2">
         <v>1.3</v>
       </c>
+      <c r="CO33" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:92">
+    <row r="34" spans="1:93">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -8199,8 +8205,9 @@
       <c r="CL34" s="15"/>
       <c r="CM34" s="15"/>
       <c r="CN34" s="15"/>
+      <c r="CO34" s="15"/>
     </row>
-    <row r="35" spans="1:92">
+    <row r="35" spans="1:93">
       <c r="BV35" s="16"/>
       <c r="BW35" s="16"/>
       <c r="BX35" s="16"/>
@@ -8209,19 +8216,19 @@
       <c r="CA35" s="16"/>
       <c r="CB35" s="16"/>
     </row>
-    <row r="36" spans="1:92">
+    <row r="36" spans="1:93">
       <c r="A36" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:92">
+    <row r="37" spans="1:93">
       <c r="A37" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:92">
+    <row r="39" spans="1:93">
       <c r="A39" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -8233,11 +8240,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:CM17"/>
+  <dimension ref="A2:CO16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="BU6" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="BZ6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="CO5" sqref="CO5:CO9"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -8250,12 +8257,12 @@
     <col min="69" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:91" ht="17.25">
+    <row r="2" spans="1:93" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:91">
+    <row r="4" spans="1:93">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -8297,7 +8304,7 @@
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
     </row>
-    <row r="5" spans="1:91">
+    <row r="5" spans="1:93">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -8568,10 +8575,16 @@
       <c r="CM5" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="CN5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="CO5" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="6" spans="1:91" ht="17.25">
+    <row r="6" spans="1:93" ht="17.25">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B6" s="5">
         <v>1.6728464306933859</v>
@@ -8843,10 +8856,16 @@
       <c r="CM6" s="2">
         <v>4</v>
       </c>
+      <c r="CN6" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="CO6" s="2">
+        <v>3.7</v>
+      </c>
     </row>
-    <row r="7" spans="1:91" ht="17.25">
+    <row r="7" spans="1:93" ht="17.25">
       <c r="A7" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B7" s="5">
         <v>1.8918263341286843</v>
@@ -9118,10 +9137,16 @@
       <c r="CM7" s="2">
         <v>4</v>
       </c>
+      <c r="CN7" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="CO7" s="2">
+        <v>3.6</v>
+      </c>
     </row>
-    <row r="8" spans="1:91" ht="17.25">
+    <row r="8" spans="1:93" ht="17.25">
       <c r="A8" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B8" s="5">
         <v>2.4902406917840634</v>
@@ -9393,10 +9418,16 @@
       <c r="CM8" s="2">
         <v>3.9</v>
       </c>
+      <c r="CN8" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="CO8" s="2">
+        <v>3.6</v>
+      </c>
     </row>
-    <row r="9" spans="1:91" ht="17.25">
+    <row r="9" spans="1:93" ht="17.25">
       <c r="A9" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B9" s="5">
         <v>2.9083419565991613</v>
@@ -9668,41 +9699,46 @@
       <c r="CM9" s="2">
         <v>3.9</v>
       </c>
+      <c r="CN9" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="CO9" s="2">
+        <v>3.6</v>
+      </c>
     </row>
-    <row r="10" spans="1:91">
+    <row r="10" spans="1:93">
       <c r="BP10" s="5"/>
     </row>
-    <row r="12" spans="1:91" ht="49.5">
+    <row r="12" spans="1:93" ht="49.5">
       <c r="A12" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:91" ht="49.5">
+    <row r="13" spans="1:93" ht="49.5">
       <c r="A13" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:91" ht="133.5">
-      <c r="A14" s="6" t="s">
-        <v>120</v>
-      </c>
+    <row r="14" spans="1:93">
+      <c r="A14" s="6"/>
     </row>
-    <row r="15" spans="1:91" ht="133.5">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:93">
+      <c r="A15" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:91">
+    <row r="16" spans="1:93">
       <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="7" t="s">
-        <v>122</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d0b21864-3105-44b5-88b9-2cedf9af7954}" enabled="1" method="Standard" siteId="{b9aaf114-bd80-4df3-b43d-ab54dd47f83f}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>